<commit_message>
Revisão dos analytic apps
Revisão dos códigos que tratam os arquivos pdf.
</commit_message>
<xml_diff>
--- a/ep_coverage.xlsx
+++ b/ep_coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7BAEE1-4F7D-4F12-856B-876A1821AB8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0591660-0852-498A-8A93-B5F3A056809B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Revisão da freight table com origem pdf
Deixei o código mais robusto a variações no pdf e extraí dele a cidade de origem, que faltava na versão anterior.
</commit_message>
<xml_diff>
--- a/ep_coverage.xlsx
+++ b/ep_coverage.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0591660-0852-498A-8A93-B5F3A056809B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B0591660-0852-498A-8A93-B5F3A056809B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="9600" windowWidth="12800" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -128,16 +128,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -435,148 +436,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>X__1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>X__11</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>gris_value</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0,30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>gris_min</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>toll_value</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4,25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>delivery_value</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>tas_value</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>other_fee_value</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>other_fee_fraction</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>cubic_factor</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>280</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>tda_value</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>tda_min</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>351,85</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>tda_max</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>882,43</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>trt_value</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>trt_min</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>isento</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>icms_tax_enable</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>iss_tax_enable</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>